<commit_message>
feat:version 1.0 of system
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chen\go\src\openscore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yang\Desktop\阅卷系统\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F4CCA5-F0F2-42B5-A193-ED90014D3784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -16204,18 +16203,18 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>22---30</t>
+    <t>87---108</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>22---31</t>
+    <t>87---109</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -16645,7 +16644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S500"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="74" workbookViewId="0">
@@ -34178,7 +34177,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K500">
+  <sortState ref="A2:K500">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -34193,11 +34192,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>

</xml_diff>